<commit_message>
Present situation this is the projectwhere it developed the exam trype
</commit_message>
<xml_diff>
--- a/Student_Results.xlsx
+++ b/Student_Results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,32 +436,32 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Name</t>
+          <t>name</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Subject1</t>
+          <t>subject1</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Subject2</t>
+          <t>subject2</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Subject3</t>
+          <t>subject3</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Total</t>
+          <t>total</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Grade</t>
+          <t>grade</t>
         </is>
       </c>
     </row>
@@ -556,6 +556,150 @@
         <v>300</v>
       </c>
       <c r="F5" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>sai</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>9</v>
+      </c>
+      <c r="C6" t="n">
+        <v>90</v>
+      </c>
+      <c r="D6" t="n">
+        <v>99</v>
+      </c>
+      <c r="E6" t="n">
+        <v>198</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Rani</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>99</v>
+      </c>
+      <c r="C7" t="n">
+        <v>99</v>
+      </c>
+      <c r="D7" t="n">
+        <v>99</v>
+      </c>
+      <c r="E7" t="n">
+        <v>297</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>rahul</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>11</v>
+      </c>
+      <c r="C8" t="n">
+        <v>11</v>
+      </c>
+      <c r="D8" t="n">
+        <v>11</v>
+      </c>
+      <c r="E8" t="n">
+        <v>33</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Rahul</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>11</v>
+      </c>
+      <c r="C9" t="n">
+        <v>12</v>
+      </c>
+      <c r="D9" t="n">
+        <v>13</v>
+      </c>
+      <c r="E9" t="n">
+        <v>36</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>rahul</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" t="n">
+        <v>3</v>
+      </c>
+      <c r="E10" t="n">
+        <v>6</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Sai</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>100</v>
+      </c>
+      <c r="C11" t="n">
+        <v>100</v>
+      </c>
+      <c r="D11" t="n">
+        <v>100</v>
+      </c>
+      <c r="E11" t="n">
+        <v>300</v>
+      </c>
+      <c r="F11" t="inlineStr">
         <is>
           <t>A</t>
         </is>

</xml_diff>